<commit_message>
Commit addition of referee columns
</commit_message>
<xml_diff>
--- a/Winning_Losing_Teams.xlsx
+++ b/Winning_Losing_Teams.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua.dipple/PycharmProjects/StatisticalDifferenceStreamlit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8788D0E2-43D3-E848-8499-5BCE7B821221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56452F0C-C61F-3D4F-A54A-892063F66ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="-22700" windowWidth="34560" windowHeight="20000" activeTab="1" xr2:uid="{31D09836-8D3C-FD4D-BFB3-8AD6B6C11E3B}"/>
+    <workbookView xWindow="-20580" yWindow="-31080" windowWidth="44480" windowHeight="21800" activeTab="1" xr2:uid="{31D09836-8D3C-FD4D-BFB3-8AD6B6C11E3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Winning Teams" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="260">
   <si>
     <r>
       <rPr>
@@ -2295,6 +2295,153 @@
   </si>
   <si>
     <t>Tier 2</t>
+  </si>
+  <si>
+    <t>Referee 1</t>
+  </si>
+  <si>
+    <t>Referee 2</t>
+  </si>
+  <si>
+    <t>Alessia Ferrari</t>
+  </si>
+  <si>
+    <t>Marta Cabanas</t>
+  </si>
+  <si>
+    <t>Andrej Franulovic</t>
+  </si>
+  <si>
+    <t>Michiel Zwart</t>
+  </si>
+  <si>
+    <t>Ivan Rakovic</t>
+  </si>
+  <si>
+    <t>Jennifer McCall</t>
+  </si>
+  <si>
+    <t>Aurely Blanchard</t>
+  </si>
+  <si>
+    <t>Nick Hodgers</t>
+  </si>
+  <si>
+    <t>Tamas Kovacs Csatlos</t>
+  </si>
+  <si>
+    <t>Boris Margeta</t>
+  </si>
+  <si>
+    <t>Frank Ohme</t>
+  </si>
+  <si>
+    <t>German Moller</t>
+  </si>
+  <si>
+    <t>Maxim Gerasimov</t>
+  </si>
+  <si>
+    <t>Liang Zhang</t>
+  </si>
+  <si>
+    <t>Fiona Haigh</t>
+  </si>
+  <si>
+    <t>Dasch Barber</t>
+  </si>
+  <si>
+    <t>Marcella Braga</t>
+  </si>
+  <si>
+    <t>Zhekang Wu</t>
+  </si>
+  <si>
+    <t>Yasser Ali</t>
+  </si>
+  <si>
+    <t>Scott Voltz</t>
+  </si>
+  <si>
+    <t>David Gomez Pordomingo</t>
+  </si>
+  <si>
+    <t>Megan Rose Perry</t>
+  </si>
+  <si>
+    <t>Chisato Kurosaki</t>
+  </si>
+  <si>
+    <t>Andrew Cairney</t>
+  </si>
+  <si>
+    <t>Jakov Blaskovic</t>
+  </si>
+  <si>
+    <t>Nicola Johnson</t>
+  </si>
+  <si>
+    <t>Natalia Markopolou</t>
+  </si>
+  <si>
+    <t>Nikolett Sajben</t>
+  </si>
+  <si>
+    <t>Matan Schwartz</t>
+  </si>
+  <si>
+    <t>Giuliana Nicolosi</t>
+  </si>
+  <si>
+    <t>Danielle Dabbaghian</t>
+  </si>
+  <si>
+    <t>Marieke van den Berg</t>
+  </si>
+  <si>
+    <t>Ruben Sap</t>
+  </si>
+  <si>
+    <t>Yuriko Udagawa</t>
+  </si>
+  <si>
+    <t>Yang Peng</t>
+  </si>
+  <si>
+    <t>Ash Kaesler</t>
+  </si>
+  <si>
+    <t>Julien Bourges</t>
+  </si>
+  <si>
+    <t>Nora Debreceni</t>
+  </si>
+  <si>
+    <t>Alessandro Severo</t>
+  </si>
+  <si>
+    <t>Georgios Kravaritis</t>
+  </si>
+  <si>
+    <t>Sebastien Dervieux</t>
+  </si>
+  <si>
+    <t>Helene Painchaud</t>
+  </si>
+  <si>
+    <t>Adrian Alexandrescu</t>
+  </si>
+  <si>
+    <t>Vojin Putnikovic</t>
+  </si>
+  <si>
+    <t>Veselin Miskovic</t>
+  </si>
+  <si>
+    <t>Georgios Stavridis</t>
+  </si>
+  <si>
+    <t>Raffaele Colombo</t>
   </si>
 </sst>
 </file>
@@ -2474,9 +2621,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{263D62CE-19FB-1D45-9D20-EC483777DAF9}" name="Table2" displayName="Table2" ref="A1:AF97" totalsRowShown="0">
-  <autoFilter ref="A1:AF97" xr:uid="{263D62CE-19FB-1D45-9D20-EC483777DAF9}"/>
-  <tableColumns count="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{263D62CE-19FB-1D45-9D20-EC483777DAF9}" name="Table2" displayName="Table2" ref="A1:AH97" totalsRowShown="0">
+  <autoFilter ref="A1:AH97" xr:uid="{263D62CE-19FB-1D45-9D20-EC483777DAF9}"/>
+  <tableColumns count="34">
     <tableColumn id="1" xr3:uid="{66FF7864-E9BB-7548-812B-B6D1506C990D}" name="Match"/>
     <tableColumn id="18" xr3:uid="{DABEAFFC-F4A3-3B4E-AFCD-0298C4C7ECFE}" name="Date"/>
     <tableColumn id="19" xr3:uid="{5924E014-4093-004F-A76E-57FB732B84A9}" name="Competition"/>
@@ -2509,6 +2656,8 @@
     <tableColumn id="31" xr3:uid="{AB83FFAF-4E5B-CF47-AC07-76AFD60D8BD1}" name="Shot Loc 4"/>
     <tableColumn id="32" xr3:uid="{272033FB-500B-E744-AAE6-7E9D4235CF5A}" name="Shot Loc 5"/>
     <tableColumn id="33" xr3:uid="{B9C7AF09-290B-1A4C-B915-9366C3D8E068}" name="Shot Loc 6"/>
+    <tableColumn id="27" xr3:uid="{6006A9B2-B356-3145-9150-AAC577958A66}" name="Referee 1"/>
+    <tableColumn id="34" xr3:uid="{BA8F68D7-1A2F-3340-8044-CC16CD90C5F3}" name="Referee 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12069,10 +12218,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FDF367E-2F8F-BD4D-A310-A68FC9A48C26}">
-  <dimension ref="A1:AG114"/>
+  <dimension ref="A1:AH114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F99" sqref="F99"/>
+      <selection activeCell="AG26" sqref="AG26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12101,10 +12250,11 @@
     <col min="25" max="25" width="26.83203125" customWidth="1"/>
     <col min="26" max="26" width="21.33203125" customWidth="1"/>
     <col min="27" max="27" width="11.33203125" customWidth="1"/>
-    <col min="28" max="33" width="11.83203125" customWidth="1"/>
+    <col min="28" max="32" width="11.83203125" customWidth="1"/>
+    <col min="33" max="34" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -12201,8 +12351,14 @@
       <c r="AF1" t="s">
         <v>58</v>
       </c>
+      <c r="AG1" t="s">
+        <v>211</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>212</v>
+      </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>157</v>
       </c>
@@ -12272,8 +12428,14 @@
       <c r="Z2">
         <v>7</v>
       </c>
+      <c r="AG2" t="s">
+        <v>213</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>253</v>
+      </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>156</v>
       </c>
@@ -12343,8 +12505,14 @@
       <c r="Z3">
         <v>7</v>
       </c>
+      <c r="AG3" t="s">
+        <v>250</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>223</v>
+      </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:34" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>153</v>
       </c>
@@ -12414,8 +12582,14 @@
       <c r="Z4">
         <v>9</v>
       </c>
+      <c r="AG4" t="s">
+        <v>254</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>226</v>
+      </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>76</v>
       </c>
@@ -12485,8 +12659,14 @@
       <c r="Z5">
         <v>10</v>
       </c>
+      <c r="AG5" t="s">
+        <v>218</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>219</v>
+      </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>151</v>
       </c>
@@ -12556,8 +12736,14 @@
       <c r="Z6">
         <v>5</v>
       </c>
+      <c r="AG6" t="s">
+        <v>250</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>220</v>
+      </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>127</v>
       </c>
@@ -12627,8 +12813,14 @@
       <c r="Z7">
         <v>14</v>
       </c>
+      <c r="AG7" t="s">
+        <v>255</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>215</v>
+      </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>149</v>
       </c>
@@ -12698,8 +12890,14 @@
       <c r="Z8">
         <v>8</v>
       </c>
+      <c r="AG8" t="s">
+        <v>213</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>235</v>
+      </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>148</v>
       </c>
@@ -12769,8 +12967,14 @@
       <c r="Z9">
         <v>8</v>
       </c>
+      <c r="AG9" t="s">
+        <v>239</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>214</v>
+      </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>113</v>
       </c>
@@ -12840,8 +13044,14 @@
       <c r="Z10">
         <v>7</v>
       </c>
+      <c r="AG10" t="s">
+        <v>222</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>223</v>
+      </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>111</v>
       </c>
@@ -12911,8 +13121,14 @@
       <c r="Z11">
         <v>9</v>
       </c>
+      <c r="AG11" t="s">
+        <v>254</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>256</v>
+      </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -12982,8 +13198,14 @@
       <c r="Z12">
         <v>11</v>
       </c>
+      <c r="AG12" t="s">
+        <v>255</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>257</v>
+      </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>109</v>
       </c>
@@ -13053,8 +13275,14 @@
       <c r="Z13">
         <v>10</v>
       </c>
+      <c r="AG13" t="s">
+        <v>213</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>258</v>
+      </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>107</v>
       </c>
@@ -13124,8 +13352,14 @@
       <c r="Z14">
         <v>5</v>
       </c>
+      <c r="AG14" t="s">
+        <v>215</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>250</v>
+      </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>105</v>
       </c>
@@ -13195,8 +13429,14 @@
       <c r="Z15">
         <v>8</v>
       </c>
+      <c r="AG15" t="s">
+        <v>257</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>220</v>
+      </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>103</v>
       </c>
@@ -13266,8 +13506,14 @@
       <c r="Z16">
         <v>3</v>
       </c>
+      <c r="AG16" t="s">
+        <v>214</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>219</v>
+      </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>101</v>
       </c>
@@ -13337,8 +13583,14 @@
       <c r="Z17">
         <v>9</v>
       </c>
+      <c r="AG17" t="s">
+        <v>215</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>223</v>
+      </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>99</v>
       </c>
@@ -13408,8 +13660,14 @@
       <c r="Z18">
         <v>12</v>
       </c>
+      <c r="AG18" t="s">
+        <v>218</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>219</v>
+      </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>97</v>
       </c>
@@ -13479,8 +13737,14 @@
       <c r="Z19">
         <v>11</v>
       </c>
+      <c r="AG19" t="s">
+        <v>256</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>257</v>
+      </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>94</v>
       </c>
@@ -13550,8 +13814,14 @@
       <c r="Z20">
         <v>9</v>
       </c>
+      <c r="AG20" t="s">
+        <v>213</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>253</v>
+      </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>92</v>
       </c>
@@ -13621,8 +13891,14 @@
       <c r="Z21">
         <v>8</v>
       </c>
+      <c r="AG21" t="s">
+        <v>256</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>226</v>
+      </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>90</v>
       </c>
@@ -13692,8 +13968,14 @@
       <c r="Z22">
         <v>9</v>
       </c>
+      <c r="AG22" t="s">
+        <v>219</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>239</v>
+      </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>87</v>
       </c>
@@ -13763,8 +14045,14 @@
       <c r="Z23">
         <v>11</v>
       </c>
+      <c r="AG23" t="s">
+        <v>218</v>
+      </c>
+      <c r="AH23" t="s">
+        <v>235</v>
+      </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -13834,8 +14122,14 @@
       <c r="Z24">
         <v>10</v>
       </c>
+      <c r="AG24" t="s">
+        <v>214</v>
+      </c>
+      <c r="AH24" t="s">
+        <v>259</v>
+      </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -13932,8 +14226,14 @@
       <c r="AF25">
         <v>4</v>
       </c>
+      <c r="AG25" t="s">
+        <v>250</v>
+      </c>
+      <c r="AH25" t="s">
+        <v>215</v>
+      </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>127</v>
       </c>
@@ -14030,8 +14330,14 @@
       <c r="AF26">
         <v>5</v>
       </c>
+      <c r="AG26" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH26" t="s">
+        <v>238</v>
+      </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>129</v>
       </c>
@@ -14128,8 +14434,14 @@
       <c r="AF27">
         <v>4</v>
       </c>
+      <c r="AG27" t="s">
+        <v>239</v>
+      </c>
+      <c r="AH27" t="s">
+        <v>240</v>
+      </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -14226,8 +14538,14 @@
       <c r="AF28">
         <v>2</v>
       </c>
+      <c r="AG28" t="s">
+        <v>241</v>
+      </c>
+      <c r="AH28" t="s">
+        <v>242</v>
+      </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>61</v>
       </c>
@@ -14324,8 +14642,14 @@
       <c r="AF29">
         <v>3</v>
       </c>
+      <c r="AG29" t="s">
+        <v>243</v>
+      </c>
+      <c r="AH29" t="s">
+        <v>223</v>
+      </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>132</v>
       </c>
@@ -14422,8 +14746,14 @@
       <c r="AF30">
         <v>5</v>
       </c>
+      <c r="AG30" t="s">
+        <v>223</v>
+      </c>
+      <c r="AH30" t="s">
+        <v>238</v>
+      </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>62</v>
       </c>
@@ -14520,8 +14850,14 @@
       <c r="AF31">
         <v>4</v>
       </c>
+      <c r="AG31" t="s">
+        <v>214</v>
+      </c>
+      <c r="AH31" t="s">
+        <v>237</v>
+      </c>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>64</v>
       </c>
@@ -14618,8 +14954,14 @@
       <c r="AF32">
         <v>9</v>
       </c>
+      <c r="AG32" t="s">
+        <v>241</v>
+      </c>
+      <c r="AH32" t="s">
+        <v>244</v>
+      </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:34" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>133</v>
       </c>
@@ -14716,8 +15058,14 @@
       <c r="AF33">
         <v>4</v>
       </c>
+      <c r="AG33" t="s">
+        <v>243</v>
+      </c>
+      <c r="AH33" t="s">
+        <v>240</v>
+      </c>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>136</v>
       </c>
@@ -14814,8 +15162,14 @@
       <c r="AF34">
         <v>1</v>
       </c>
+      <c r="AG34" t="s">
+        <v>243</v>
+      </c>
+      <c r="AH34" t="s">
+        <v>214</v>
+      </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>137</v>
       </c>
@@ -14912,8 +15266,14 @@
       <c r="AF35">
         <v>2</v>
       </c>
+      <c r="AG35" t="s">
+        <v>223</v>
+      </c>
+      <c r="AH35" t="s">
+        <v>244</v>
+      </c>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -15010,8 +15370,14 @@
       <c r="AF36">
         <v>1</v>
       </c>
+      <c r="AG36" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH36" t="s">
+        <v>239</v>
+      </c>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>140</v>
       </c>
@@ -15108,8 +15474,14 @@
       <c r="AF37">
         <v>1</v>
       </c>
+      <c r="AG37" t="s">
+        <v>244</v>
+      </c>
+      <c r="AH37" t="s">
+        <v>214</v>
+      </c>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>141</v>
       </c>
@@ -15206,8 +15578,14 @@
       <c r="AF38">
         <v>3</v>
       </c>
+      <c r="AG38" t="s">
+        <v>238</v>
+      </c>
+      <c r="AH38" t="s">
+        <v>223</v>
+      </c>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>66</v>
       </c>
@@ -15304,8 +15682,14 @@
       <c r="AF39">
         <v>4</v>
       </c>
+      <c r="AG39" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH39" t="s">
+        <v>242</v>
+      </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>67</v>
       </c>
@@ -15402,8 +15786,14 @@
       <c r="AF40">
         <v>6</v>
       </c>
+      <c r="AG40" t="s">
+        <v>241</v>
+      </c>
+      <c r="AH40" t="s">
+        <v>240</v>
+      </c>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>143</v>
       </c>
@@ -15500,8 +15890,14 @@
       <c r="AF41">
         <v>9</v>
       </c>
+      <c r="AG41" t="s">
+        <v>244</v>
+      </c>
+      <c r="AH41" t="s">
+        <v>239</v>
+      </c>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>68</v>
       </c>
@@ -15598,8 +15994,14 @@
       <c r="AF42">
         <v>2</v>
       </c>
+      <c r="AG42" t="s">
+        <v>214</v>
+      </c>
+      <c r="AH42" t="s">
+        <v>237</v>
+      </c>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>69</v>
       </c>
@@ -15696,8 +16098,14 @@
       <c r="AF43">
         <v>1</v>
       </c>
+      <c r="AG43" t="s">
+        <v>241</v>
+      </c>
+      <c r="AH43" t="s">
+        <v>243</v>
+      </c>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>70</v>
       </c>
@@ -15794,8 +16202,14 @@
       <c r="AF44">
         <v>5</v>
       </c>
+      <c r="AG44" t="s">
+        <v>242</v>
+      </c>
+      <c r="AH44" t="s">
+        <v>223</v>
+      </c>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>129</v>
       </c>
@@ -15892,8 +16306,14 @@
       <c r="AF45">
         <v>7</v>
       </c>
+      <c r="AG45" t="s">
+        <v>238</v>
+      </c>
+      <c r="AH45" t="s">
+        <v>214</v>
+      </c>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>145</v>
       </c>
@@ -15990,8 +16410,14 @@
       <c r="AF46">
         <v>1</v>
       </c>
+      <c r="AG46" t="s">
+        <v>239</v>
+      </c>
+      <c r="AH46" t="s">
+        <v>237</v>
+      </c>
     </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>61</v>
       </c>
@@ -16088,8 +16514,14 @@
       <c r="AF47">
         <v>2</v>
       </c>
+      <c r="AG47" t="s">
+        <v>241</v>
+      </c>
+      <c r="AH47" t="s">
+        <v>242</v>
+      </c>
     </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>71</v>
       </c>
@@ -16186,8 +16618,14 @@
       <c r="AF48">
         <v>5</v>
       </c>
+      <c r="AG48" t="s">
+        <v>223</v>
+      </c>
+      <c r="AH48" t="s">
+        <v>240</v>
+      </c>
     </row>
-    <row r="49" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>72</v>
       </c>
@@ -16284,8 +16722,14 @@
       <c r="AF49">
         <v>3</v>
       </c>
+      <c r="AG49" t="s">
+        <v>245</v>
+      </c>
+      <c r="AH49" t="s">
+        <v>246</v>
+      </c>
     </row>
-    <row r="50" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>119</v>
       </c>
@@ -16382,8 +16826,14 @@
       <c r="AF50">
         <v>3</v>
       </c>
+      <c r="AG50" t="s">
+        <v>247</v>
+      </c>
+      <c r="AH50" t="s">
+        <v>248</v>
+      </c>
     </row>
-    <row r="51" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>74</v>
       </c>
@@ -16480,8 +16930,14 @@
       <c r="AF51">
         <v>8</v>
       </c>
+      <c r="AG51" t="s">
+        <v>249</v>
+      </c>
+      <c r="AH51" t="s">
+        <v>250</v>
+      </c>
     </row>
-    <row r="52" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>75</v>
       </c>
@@ -16578,8 +17034,14 @@
       <c r="AF52">
         <v>2</v>
       </c>
+      <c r="AG52" t="s">
+        <v>218</v>
+      </c>
+      <c r="AH52" t="s">
+        <v>251</v>
+      </c>
     </row>
-    <row r="53" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>123</v>
       </c>
@@ -16676,8 +17138,14 @@
       <c r="AF53">
         <v>3</v>
       </c>
+      <c r="AG53" t="s">
+        <v>252</v>
+      </c>
+      <c r="AH53" t="s">
+        <v>245</v>
+      </c>
     </row>
-    <row r="54" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>76</v>
       </c>
@@ -16774,8 +17242,14 @@
       <c r="AF54">
         <v>4</v>
       </c>
+      <c r="AG54" t="s">
+        <v>214</v>
+      </c>
+      <c r="AH54" t="s">
+        <v>250</v>
+      </c>
     </row>
-    <row r="55" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>77</v>
       </c>
@@ -16872,8 +17346,14 @@
       <c r="AF55">
         <v>2</v>
       </c>
+      <c r="AG55" t="s">
+        <v>251</v>
+      </c>
+      <c r="AH55" t="s">
+        <v>218</v>
+      </c>
     </row>
-    <row r="56" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>78</v>
       </c>
@@ -16970,8 +17450,14 @@
       <c r="AF56">
         <v>5</v>
       </c>
+      <c r="AG56" t="s">
+        <v>249</v>
+      </c>
+      <c r="AH56" t="s">
+        <v>248</v>
+      </c>
     </row>
-    <row r="57" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>124</v>
       </c>
@@ -17068,8 +17554,14 @@
       <c r="AF57">
         <v>0</v>
       </c>
+      <c r="AG57" t="s">
+        <v>218</v>
+      </c>
+      <c r="AH57" t="s">
+        <v>248</v>
+      </c>
     </row>
-    <row r="58" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>79</v>
       </c>
@@ -17166,8 +17658,14 @@
       <c r="AF58">
         <v>5</v>
       </c>
+      <c r="AG58" t="s">
+        <v>252</v>
+      </c>
+      <c r="AH58" t="s">
+        <v>250</v>
+      </c>
     </row>
-    <row r="59" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>80</v>
       </c>
@@ -17264,8 +17762,14 @@
       <c r="AF59">
         <v>3</v>
       </c>
+      <c r="AG59" t="s">
+        <v>251</v>
+      </c>
+      <c r="AH59" t="s">
+        <v>214</v>
+      </c>
     </row>
-    <row r="60" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>161</v>
       </c>
@@ -17363,7 +17867,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>66</v>
       </c>
@@ -17461,7 +17965,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>164</v>
       </c>
@@ -17559,7 +18063,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>166</v>
       </c>
@@ -17657,7 +18161,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>168</v>
       </c>
@@ -17755,7 +18259,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>170</v>
       </c>
@@ -17853,7 +18357,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>173</v>
       </c>
@@ -17950,8 +18454,14 @@
       <c r="AF66">
         <v>7</v>
       </c>
+      <c r="AG66" t="s">
+        <v>227</v>
+      </c>
+      <c r="AH66" t="s">
+        <v>236</v>
+      </c>
     </row>
-    <row r="67" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -18048,8 +18558,14 @@
       <c r="AF67">
         <v>4</v>
       </c>
+      <c r="AG67" t="s">
+        <v>227</v>
+      </c>
+      <c r="AH67" t="s">
+        <v>236</v>
+      </c>
     </row>
-    <row r="68" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>174</v>
       </c>
@@ -18146,8 +18662,14 @@
       <c r="AF68">
         <v>7</v>
       </c>
+      <c r="AG68" t="s">
+        <v>214</v>
+      </c>
+      <c r="AH68" t="s">
+        <v>235</v>
+      </c>
     </row>
-    <row r="69" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>177</v>
       </c>
@@ -18244,8 +18766,14 @@
       <c r="AF69">
         <v>4</v>
       </c>
+      <c r="AG69" t="s">
+        <v>213</v>
+      </c>
+      <c r="AH69" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="70" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>179</v>
       </c>
@@ -18342,8 +18870,14 @@
       <c r="AF70">
         <v>3</v>
       </c>
+      <c r="AG70" t="s">
+        <v>227</v>
+      </c>
+      <c r="AH70" t="s">
+        <v>226</v>
+      </c>
     </row>
-    <row r="71" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>181</v>
       </c>
@@ -18440,8 +18974,14 @@
       <c r="AF71">
         <v>7</v>
       </c>
+      <c r="AG71" t="s">
+        <v>219</v>
+      </c>
+      <c r="AH71" t="s">
+        <v>221</v>
+      </c>
     </row>
-    <row r="72" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>182</v>
       </c>
@@ -18538,8 +19078,14 @@
       <c r="AF72">
         <v>3</v>
       </c>
+      <c r="AG72" t="s">
+        <v>229</v>
+      </c>
+      <c r="AH72" t="s">
+        <v>222</v>
+      </c>
     </row>
-    <row r="73" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>184</v>
       </c>
@@ -18636,8 +19182,14 @@
       <c r="AF73">
         <v>5</v>
       </c>
+      <c r="AG73" t="s">
+        <v>218</v>
+      </c>
+      <c r="AH73" t="s">
+        <v>223</v>
+      </c>
     </row>
-    <row r="74" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>185</v>
       </c>
@@ -18734,8 +19286,14 @@
       <c r="AF74">
         <v>4</v>
       </c>
+      <c r="AG74" t="s">
+        <v>224</v>
+      </c>
+      <c r="AH74" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="75" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>186</v>
       </c>
@@ -18832,8 +19390,14 @@
       <c r="AF75">
         <v>5</v>
       </c>
+      <c r="AG75" t="s">
+        <v>213</v>
+      </c>
+      <c r="AH75" t="s">
+        <v>217</v>
+      </c>
     </row>
-    <row r="76" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>187</v>
       </c>
@@ -18930,8 +19494,14 @@
       <c r="AF76">
         <v>7</v>
       </c>
+      <c r="AG76" t="s">
+        <v>218</v>
+      </c>
+      <c r="AH76" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="77" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>188</v>
       </c>
@@ -19028,8 +19598,14 @@
       <c r="AF77">
         <v>5</v>
       </c>
+      <c r="AG77" t="s">
+        <v>233</v>
+      </c>
+      <c r="AH77" t="s">
+        <v>223</v>
+      </c>
     </row>
-    <row r="78" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>189</v>
       </c>
@@ -19126,8 +19702,14 @@
       <c r="AF78">
         <v>5</v>
       </c>
+      <c r="AG78" t="s">
+        <v>219</v>
+      </c>
+      <c r="AH78" t="s">
+        <v>222</v>
+      </c>
     </row>
-    <row r="79" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>190</v>
       </c>
@@ -19224,8 +19806,14 @@
       <c r="AF79">
         <v>3</v>
       </c>
+      <c r="AG79" t="s">
+        <v>230</v>
+      </c>
+      <c r="AH79" t="s">
+        <v>232</v>
+      </c>
     </row>
-    <row r="80" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>191</v>
       </c>
@@ -19322,8 +19910,14 @@
       <c r="AF80">
         <v>7</v>
       </c>
+      <c r="AG80" t="s">
+        <v>215</v>
+      </c>
+      <c r="AH80" t="s">
+        <v>231</v>
+      </c>
     </row>
-    <row r="81" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>192</v>
       </c>
@@ -19420,8 +20014,14 @@
       <c r="AF81">
         <v>4</v>
       </c>
+      <c r="AG81" t="s">
+        <v>221</v>
+      </c>
+      <c r="AH81" t="s">
+        <v>214</v>
+      </c>
     </row>
-    <row r="82" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>193</v>
       </c>
@@ -19518,8 +20118,14 @@
       <c r="AF82">
         <v>8</v>
       </c>
+      <c r="AG82" t="s">
+        <v>218</v>
+      </c>
+      <c r="AH82" t="s">
+        <v>214</v>
+      </c>
     </row>
-    <row r="83" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>194</v>
       </c>
@@ -19616,8 +20222,14 @@
       <c r="AF83">
         <v>5</v>
       </c>
+      <c r="AG83" t="s">
+        <v>230</v>
+      </c>
+      <c r="AH83" t="s">
+        <v>224</v>
+      </c>
     </row>
-    <row r="84" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>195</v>
       </c>
@@ -19714,8 +20326,14 @@
       <c r="AF84">
         <v>6</v>
       </c>
+      <c r="AG84" t="s">
+        <v>228</v>
+      </c>
+      <c r="AH84" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="85" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>196</v>
       </c>
@@ -19812,8 +20430,14 @@
       <c r="AF85">
         <v>4</v>
       </c>
+      <c r="AG85" t="s">
+        <v>219</v>
+      </c>
+      <c r="AH85" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="86" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>197</v>
       </c>
@@ -19910,8 +20534,14 @@
       <c r="AF86">
         <v>3</v>
       </c>
+      <c r="AG86" t="s">
+        <v>226</v>
+      </c>
+      <c r="AH86" t="s">
+        <v>216</v>
+      </c>
     </row>
-    <row r="87" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>198</v>
       </c>
@@ -20008,8 +20638,14 @@
       <c r="AF87">
         <v>8</v>
       </c>
+      <c r="AG87" t="s">
+        <v>213</v>
+      </c>
+      <c r="AH87" t="s">
+        <v>214</v>
+      </c>
     </row>
-    <row r="88" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>199</v>
       </c>
@@ -20106,8 +20742,14 @@
       <c r="AF88">
         <v>4</v>
       </c>
+      <c r="AG88" t="s">
+        <v>218</v>
+      </c>
+      <c r="AH88" t="s">
+        <v>222</v>
+      </c>
     </row>
-    <row r="89" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>200</v>
       </c>
@@ -20204,8 +20846,14 @@
       <c r="AF89">
         <v>4</v>
       </c>
+      <c r="AG89" t="s">
+        <v>219</v>
+      </c>
+      <c r="AH89" t="s">
+        <v>225</v>
+      </c>
     </row>
-    <row r="90" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>201</v>
       </c>
@@ -20302,8 +20950,14 @@
       <c r="AF90">
         <v>3</v>
       </c>
+      <c r="AG90" t="s">
+        <v>218</v>
+      </c>
+      <c r="AH90" t="s">
+        <v>224</v>
+      </c>
     </row>
-    <row r="91" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>202</v>
       </c>
@@ -20400,8 +21054,14 @@
       <c r="AF91">
         <v>2</v>
       </c>
+      <c r="AG91" t="s">
+        <v>222</v>
+      </c>
+      <c r="AH91" t="s">
+        <v>223</v>
+      </c>
     </row>
-    <row r="92" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>203</v>
       </c>
@@ -20498,8 +21158,14 @@
       <c r="AF92">
         <v>4</v>
       </c>
+      <c r="AG92" t="s">
+        <v>221</v>
+      </c>
+      <c r="AH92" t="s">
+        <v>214</v>
+      </c>
     </row>
-    <row r="93" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>204</v>
       </c>
@@ -20596,8 +21262,14 @@
       <c r="AF93">
         <v>6</v>
       </c>
+      <c r="AG93" t="s">
+        <v>213</v>
+      </c>
+      <c r="AH93" t="s">
+        <v>215</v>
+      </c>
     </row>
-    <row r="94" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>205</v>
       </c>
@@ -20694,8 +21366,14 @@
       <c r="AF94">
         <v>5</v>
       </c>
+      <c r="AG94" t="s">
+        <v>219</v>
+      </c>
+      <c r="AH94" t="s">
+        <v>220</v>
+      </c>
     </row>
-    <row r="95" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>206</v>
       </c>
@@ -20792,8 +21470,14 @@
       <c r="AF95">
         <v>4</v>
       </c>
+      <c r="AG95" t="s">
+        <v>215</v>
+      </c>
+      <c r="AH95" t="s">
+        <v>216</v>
+      </c>
     </row>
-    <row r="96" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>207</v>
       </c>
@@ -20890,8 +21574,14 @@
       <c r="AF96">
         <v>4</v>
       </c>
+      <c r="AG96" t="s">
+        <v>217</v>
+      </c>
+      <c r="AH96" t="s">
+        <v>218</v>
+      </c>
     </row>
-    <row r="97" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>184</v>
       </c>
@@ -20988,8 +21678,14 @@
       <c r="AF97">
         <v>1</v>
       </c>
+      <c r="AG97" t="s">
+        <v>213</v>
+      </c>
+      <c r="AH97" t="s">
+        <v>214</v>
+      </c>
     </row>
-    <row r="100" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>25</v>
       </c>
@@ -21106,7 +21802,7 @@
         <v>4.1967213114754101</v>
       </c>
     </row>
-    <row r="101" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>26</v>
       </c>
@@ -21182,7 +21878,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="102" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:34" x14ac:dyDescent="0.2">
       <c r="H102" s="2">
         <f>H101/(H101+I101+J101)</f>
         <v>0.481941309255079</v>
@@ -21244,13 +21940,13 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="106" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:34" x14ac:dyDescent="0.2">
       <c r="S106" s="11" t="s">
         <v>81</v>
       </c>
       <c r="T106" s="11"/>
     </row>
-    <row r="107" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:34" x14ac:dyDescent="0.2">
       <c r="S107" s="11"/>
       <c r="T107" s="11"/>
     </row>

</xml_diff>

<commit_message>
Commit referee analysis tab
</commit_message>
<xml_diff>
--- a/Winning_Losing_Teams.xlsx
+++ b/Winning_Losing_Teams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua.dipple/PycharmProjects/StatisticalDifferenceStreamlit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56452F0C-C61F-3D4F-A54A-892063F66ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518C33DC-A24C-9B47-B5B4-B8697BEF09C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20580" yWindow="-31080" windowWidth="44480" windowHeight="21800" activeTab="1" xr2:uid="{31D09836-8D3C-FD4D-BFB3-8AD6B6C11E3B}"/>
+    <workbookView xWindow="-20580" yWindow="-31080" windowWidth="44480" windowHeight="21800" xr2:uid="{31D09836-8D3C-FD4D-BFB3-8AD6B6C11E3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Winning Teams" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="260">
   <si>
     <r>
       <rPr>
@@ -2519,7 +2519,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -2538,12 +2538,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF44B3E1"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF44B3E1"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF44B3E1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -2561,6 +2574,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2580,9 +2595,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FAF07BB7-650B-FB4C-B20B-F4DC341A3990}" name="Table1" displayName="Table1" ref="A1:AF97" totalsRowShown="0">
-  <autoFilter ref="A1:AF97" xr:uid="{FAF07BB7-650B-FB4C-B20B-F4DC341A3990}"/>
-  <tableColumns count="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FAF07BB7-650B-FB4C-B20B-F4DC341A3990}" name="Table1" displayName="Table1" ref="A1:AH97" totalsRowShown="0">
+  <autoFilter ref="A1:AH97" xr:uid="{FAF07BB7-650B-FB4C-B20B-F4DC341A3990}"/>
+  <tableColumns count="34">
     <tableColumn id="1" xr3:uid="{B0F85548-0EDE-8C4B-BB18-BD50D477EDBD}" name="Match"/>
     <tableColumn id="19" xr3:uid="{28B3E851-942C-3A47-B058-39094C7137E2}" name="Date"/>
     <tableColumn id="18" xr3:uid="{CA0FB440-BD88-5343-ABBC-08542D8EF4EE}" name="Competition"/>
@@ -2615,6 +2630,8 @@
     <tableColumn id="31" xr3:uid="{93B1DB13-F410-5542-98F6-36121A7CD7F4}" name="Shot Loc 4"/>
     <tableColumn id="32" xr3:uid="{CA4488F7-65FA-AA4E-9F3E-A1868F0C1386}" name="Shot Loc 5"/>
     <tableColumn id="33" xr3:uid="{234AFD40-3C96-FA45-9A47-31403D6F625B}" name="Shot Loc 6"/>
+    <tableColumn id="27" xr3:uid="{98587882-C493-E443-AB52-5CAAC876F44A}" name="Referee 1"/>
+    <tableColumn id="34" xr3:uid="{954ECC6B-FAF2-7847-A7D1-B99D75D4C4B8}" name="Referee 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2980,10 +2997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8145AF1-11A6-9D49-88E0-C1A7D6AB31B7}">
-  <dimension ref="A1:AG113"/>
+  <dimension ref="A1:AH113"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F99" sqref="F99"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH14" sqref="AH14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3012,10 +3029,12 @@
     <col min="25" max="25" width="21.1640625" customWidth="1"/>
     <col min="26" max="26" width="11.83203125" customWidth="1"/>
     <col min="27" max="27" width="13.33203125" customWidth="1"/>
-    <col min="28" max="33" width="11.83203125" customWidth="1"/>
+    <col min="28" max="32" width="11.83203125" customWidth="1"/>
+    <col min="33" max="33" width="22" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -3112,8 +3131,14 @@
       <c r="AF1" t="s">
         <v>58</v>
       </c>
+      <c r="AG1" t="s">
+        <v>211</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>212</v>
+      </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>158</v>
       </c>
@@ -3183,8 +3208,14 @@
       <c r="Z2">
         <v>5</v>
       </c>
+      <c r="AG2" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="AH2" s="13" t="s">
+        <v>253</v>
+      </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>155</v>
       </c>
@@ -3254,8 +3285,14 @@
       <c r="Z3">
         <v>12</v>
       </c>
+      <c r="AG3" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="AH3" s="14" t="s">
+        <v>223</v>
+      </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>154</v>
       </c>
@@ -3325,8 +3362,14 @@
       <c r="Z4">
         <v>10</v>
       </c>
+      <c r="AG4" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="AH4" s="13" t="s">
+        <v>226</v>
+      </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -3396,8 +3439,14 @@
       <c r="Z5">
         <v>5</v>
       </c>
+      <c r="AG5" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="AH5" s="14" t="s">
+        <v>219</v>
+      </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>152</v>
       </c>
@@ -3467,8 +3516,14 @@
       <c r="Z6">
         <v>14</v>
       </c>
+      <c r="AG6" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="AH6" s="13" t="s">
+        <v>220</v>
+      </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>126</v>
       </c>
@@ -3538,8 +3593,14 @@
       <c r="Z7">
         <v>8</v>
       </c>
+      <c r="AG7" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="AH7" s="14" t="s">
+        <v>215</v>
+      </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>150</v>
       </c>
@@ -3609,8 +3670,14 @@
       <c r="Z8">
         <v>9</v>
       </c>
+      <c r="AG8" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="AH8" s="13" t="s">
+        <v>235</v>
+      </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>147</v>
       </c>
@@ -3680,8 +3747,14 @@
       <c r="Z9">
         <v>8</v>
       </c>
+      <c r="AG9" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="AH9" s="14" t="s">
+        <v>214</v>
+      </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>112</v>
       </c>
@@ -3751,8 +3824,14 @@
       <c r="Z10">
         <v>9</v>
       </c>
+      <c r="AG10" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="AH10" s="13" t="s">
+        <v>223</v>
+      </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>110</v>
       </c>
@@ -3822,8 +3901,14 @@
       <c r="Z11">
         <v>10</v>
       </c>
+      <c r="AG11" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="AH11" s="14" t="s">
+        <v>256</v>
+      </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -3893,8 +3978,14 @@
       <c r="Z12">
         <v>11</v>
       </c>
+      <c r="AG12" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="AH12" s="13" t="s">
+        <v>257</v>
+      </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>108</v>
       </c>
@@ -3964,8 +4055,14 @@
       <c r="Z13">
         <v>6</v>
       </c>
+      <c r="AG13" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="AH13" s="14" t="s">
+        <v>258</v>
+      </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>106</v>
       </c>
@@ -4035,8 +4132,14 @@
       <c r="Z14">
         <v>7</v>
       </c>
+      <c r="AG14" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="AH14" s="13" t="s">
+        <v>250</v>
+      </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>104</v>
       </c>
@@ -4106,8 +4209,14 @@
       <c r="Z15">
         <v>12</v>
       </c>
+      <c r="AG15" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="AH15" s="14" t="s">
+        <v>220</v>
+      </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>102</v>
       </c>
@@ -4177,8 +4286,14 @@
       <c r="Z16">
         <v>7</v>
       </c>
+      <c r="AG16" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="AH16" s="13" t="s">
+        <v>219</v>
+      </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>100</v>
       </c>
@@ -4248,8 +4363,14 @@
       <c r="Z17">
         <v>11</v>
       </c>
+      <c r="AG17" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="AH17" s="14" t="s">
+        <v>223</v>
+      </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>98</v>
       </c>
@@ -4319,8 +4440,14 @@
       <c r="Z18">
         <v>9</v>
       </c>
+      <c r="AG18" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="AH18" s="13" t="s">
+        <v>219</v>
+      </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>95</v>
       </c>
@@ -4390,8 +4517,14 @@
       <c r="Z19">
         <v>10</v>
       </c>
+      <c r="AG19" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="AH19" s="14" t="s">
+        <v>257</v>
+      </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>93</v>
       </c>
@@ -4461,8 +4594,14 @@
       <c r="Z20">
         <v>13</v>
       </c>
+      <c r="AG20" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="AH20" s="13" t="s">
+        <v>253</v>
+      </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>91</v>
       </c>
@@ -4532,8 +4671,14 @@
       <c r="Z21">
         <v>16</v>
       </c>
+      <c r="AG21" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="AH21" s="14" t="s">
+        <v>226</v>
+      </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>89</v>
       </c>
@@ -4603,8 +4748,14 @@
       <c r="Z22">
         <v>13</v>
       </c>
+      <c r="AG22" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="AH22" s="13" t="s">
+        <v>239</v>
+      </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>86</v>
       </c>
@@ -4674,8 +4825,14 @@
       <c r="Z23">
         <v>10</v>
       </c>
+      <c r="AG23" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="AH23" s="14" t="s">
+        <v>235</v>
+      </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>83</v>
       </c>
@@ -4745,8 +4902,14 @@
       <c r="Z24">
         <v>10</v>
       </c>
+      <c r="AG24" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="AH24" s="13" t="s">
+        <v>259</v>
+      </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -4843,8 +5006,14 @@
       <c r="AF25">
         <v>7</v>
       </c>
+      <c r="AG25" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="AH25" s="14" t="s">
+        <v>215</v>
+      </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>126</v>
       </c>
@@ -4941,8 +5110,14 @@
       <c r="AF26">
         <v>3</v>
       </c>
+      <c r="AG26" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH26" s="13" t="s">
+        <v>238</v>
+      </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>130</v>
       </c>
@@ -5039,8 +5214,14 @@
       <c r="AF27">
         <v>1</v>
       </c>
+      <c r="AG27" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="AH27" s="14" t="s">
+        <v>240</v>
+      </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -5137,8 +5318,14 @@
       <c r="AF28">
         <v>4</v>
       </c>
+      <c r="AG28" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="AH28" s="13" t="s">
+        <v>242</v>
+      </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -5235,8 +5422,14 @@
       <c r="AF29">
         <v>4</v>
       </c>
+      <c r="AG29" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="AH29" s="14" t="s">
+        <v>223</v>
+      </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>131</v>
       </c>
@@ -5333,8 +5526,14 @@
       <c r="AF30">
         <v>3</v>
       </c>
+      <c r="AG30" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="AH30" s="13" t="s">
+        <v>238</v>
+      </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -5431,8 +5630,14 @@
       <c r="AF31">
         <v>6</v>
       </c>
+      <c r="AG31" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="AH31" s="14" t="s">
+        <v>237</v>
+      </c>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -5529,8 +5734,14 @@
       <c r="AF32">
         <v>5</v>
       </c>
+      <c r="AG32" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="AH32" s="13" t="s">
+        <v>244</v>
+      </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>134</v>
       </c>
@@ -5627,8 +5838,14 @@
       <c r="AF33">
         <v>1</v>
       </c>
+      <c r="AG33" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="AH33" s="14" t="s">
+        <v>240</v>
+      </c>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>135</v>
       </c>
@@ -5725,8 +5942,14 @@
       <c r="AF34">
         <v>0</v>
       </c>
+      <c r="AG34" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="AH34" s="13" t="s">
+        <v>214</v>
+      </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>138</v>
       </c>
@@ -5823,8 +6046,14 @@
       <c r="AF35">
         <v>4</v>
       </c>
+      <c r="AG35" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="AH35" s="14" t="s">
+        <v>244</v>
+      </c>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -5921,8 +6150,14 @@
       <c r="AF36">
         <v>1</v>
       </c>
+      <c r="AG36" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH36" s="13" t="s">
+        <v>239</v>
+      </c>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>139</v>
       </c>
@@ -6019,8 +6254,14 @@
       <c r="AF37">
         <v>4</v>
       </c>
+      <c r="AG37" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="AH37" s="14" t="s">
+        <v>214</v>
+      </c>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>142</v>
       </c>
@@ -6117,8 +6358,14 @@
       <c r="AF38">
         <v>8</v>
       </c>
+      <c r="AG38" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="AH38" s="13" t="s">
+        <v>223</v>
+      </c>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -6215,8 +6462,14 @@
       <c r="AF39">
         <v>3</v>
       </c>
+      <c r="AG39" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH39" s="14" t="s">
+        <v>242</v>
+      </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -6313,8 +6566,14 @@
       <c r="AF40">
         <v>6</v>
       </c>
+      <c r="AG40" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="AH40" s="13" t="s">
+        <v>240</v>
+      </c>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>144</v>
       </c>
@@ -6411,8 +6670,14 @@
       <c r="AF41">
         <v>0</v>
       </c>
+      <c r="AG41" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="AH41" s="14" t="s">
+        <v>239</v>
+      </c>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -6509,8 +6774,14 @@
       <c r="AF42">
         <v>3</v>
       </c>
+      <c r="AG42" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="AH42" s="13" t="s">
+        <v>237</v>
+      </c>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -6607,8 +6878,14 @@
       <c r="AF43">
         <v>11</v>
       </c>
+      <c r="AG43" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="AH43" s="14" t="s">
+        <v>243</v>
+      </c>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>15</v>
       </c>
@@ -6705,8 +6982,14 @@
       <c r="AF44">
         <v>2</v>
       </c>
+      <c r="AG44" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="AH44" s="13" t="s">
+        <v>223</v>
+      </c>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>130</v>
       </c>
@@ -6803,8 +7086,14 @@
       <c r="AF45">
         <v>2</v>
       </c>
+      <c r="AG45" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="AH45" s="14" t="s">
+        <v>214</v>
+      </c>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>146</v>
       </c>
@@ -6901,8 +7190,14 @@
       <c r="AF46">
         <v>6</v>
       </c>
+      <c r="AG46" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="AH46" s="13" t="s">
+        <v>237</v>
+      </c>
     </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -6999,8 +7294,14 @@
       <c r="AF47">
         <v>3</v>
       </c>
+      <c r="AG47" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="AH47" s="14" t="s">
+        <v>242</v>
+      </c>
     </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>16</v>
       </c>
@@ -7097,8 +7398,14 @@
       <c r="AF48">
         <v>1</v>
       </c>
+      <c r="AG48" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="AH48" s="13" t="s">
+        <v>240</v>
+      </c>
     </row>
-    <row r="49" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>17</v>
       </c>
@@ -7195,8 +7502,14 @@
       <c r="AF49">
         <v>4</v>
       </c>
+      <c r="AG49" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="AH49" s="14" t="s">
+        <v>246</v>
+      </c>
     </row>
-    <row r="50" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>121</v>
       </c>
@@ -7293,8 +7606,14 @@
       <c r="AF50">
         <v>2</v>
       </c>
+      <c r="AG50" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="AH50" s="13" t="s">
+        <v>248</v>
+      </c>
     </row>
-    <row r="51" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>18</v>
       </c>
@@ -7391,8 +7710,14 @@
       <c r="AF51">
         <v>4</v>
       </c>
+      <c r="AG51" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="AH51" s="14" t="s">
+        <v>250</v>
+      </c>
     </row>
-    <row r="52" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>19</v>
       </c>
@@ -7489,8 +7814,14 @@
       <c r="AF52">
         <v>6</v>
       </c>
+      <c r="AG52" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="AH52" s="13" t="s">
+        <v>251</v>
+      </c>
     </row>
-    <row r="53" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>122</v>
       </c>
@@ -7587,8 +7918,14 @@
       <c r="AF53">
         <v>3</v>
       </c>
+      <c r="AG53" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="AH53" s="14" t="s">
+        <v>245</v>
+      </c>
     </row>
-    <row r="54" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>20</v>
       </c>
@@ -7685,8 +8022,14 @@
       <c r="AF54">
         <v>1</v>
       </c>
+      <c r="AG54" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="AH54" s="13" t="s">
+        <v>250</v>
+      </c>
     </row>
-    <row r="55" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>21</v>
       </c>
@@ -7783,8 +8126,14 @@
       <c r="AF55">
         <v>3</v>
       </c>
+      <c r="AG55" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="AH55" s="14" t="s">
+        <v>218</v>
+      </c>
     </row>
-    <row r="56" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>22</v>
       </c>
@@ -7881,8 +8230,14 @@
       <c r="AF56">
         <v>4</v>
       </c>
+      <c r="AG56" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="AH56" s="13" t="s">
+        <v>248</v>
+      </c>
     </row>
-    <row r="57" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>125</v>
       </c>
@@ -7979,8 +8334,14 @@
       <c r="AF57">
         <v>4</v>
       </c>
+      <c r="AG57" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="AH57" s="14" t="s">
+        <v>248</v>
+      </c>
     </row>
-    <row r="58" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>23</v>
       </c>
@@ -8077,8 +8438,14 @@
       <c r="AF58">
         <v>0</v>
       </c>
+      <c r="AG58" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="AH58" s="13" t="s">
+        <v>250</v>
+      </c>
     </row>
-    <row r="59" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>24</v>
       </c>
@@ -8175,8 +8542,14 @@
       <c r="AF59">
         <v>8</v>
       </c>
+      <c r="AG59" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="AH59" s="14" t="s">
+        <v>214</v>
+      </c>
     </row>
-    <row r="60" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>160</v>
       </c>
@@ -8273,8 +8646,10 @@
       <c r="AF60">
         <v>3</v>
       </c>
+      <c r="AG60" s="6"/>
+      <c r="AH60" s="13"/>
     </row>
-    <row r="61" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>10</v>
       </c>
@@ -8371,8 +8746,10 @@
       <c r="AF61">
         <v>2</v>
       </c>
+      <c r="AG61" s="8"/>
+      <c r="AH61" s="14"/>
     </row>
-    <row r="62" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>163</v>
       </c>
@@ -8469,8 +8846,10 @@
       <c r="AF62">
         <v>3</v>
       </c>
+      <c r="AG62" s="6"/>
+      <c r="AH62" s="13"/>
     </row>
-    <row r="63" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>165</v>
       </c>
@@ -8567,8 +8946,10 @@
       <c r="AF63">
         <v>3</v>
       </c>
+      <c r="AG63" s="8"/>
+      <c r="AH63" s="14"/>
     </row>
-    <row r="64" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>167</v>
       </c>
@@ -8665,8 +9046,10 @@
       <c r="AF64">
         <v>2</v>
       </c>
+      <c r="AG64" s="6"/>
+      <c r="AH64" s="13"/>
     </row>
-    <row r="65" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>169</v>
       </c>
@@ -8763,8 +9146,10 @@
       <c r="AF65">
         <v>3</v>
       </c>
+      <c r="AG65" s="8"/>
+      <c r="AH65" s="14"/>
     </row>
-    <row r="66" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>172</v>
       </c>
@@ -8861,8 +9246,14 @@
       <c r="AF66">
         <v>7</v>
       </c>
+      <c r="AG66" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="AH66" s="13" t="s">
+        <v>236</v>
+      </c>
     </row>
-    <row r="67" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>8</v>
       </c>
@@ -8959,8 +9350,14 @@
       <c r="AF67">
         <v>5</v>
       </c>
+      <c r="AG67" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="AH67" s="14" t="s">
+        <v>236</v>
+      </c>
     </row>
-    <row r="68" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>175</v>
       </c>
@@ -9057,8 +9454,14 @@
       <c r="AF68">
         <v>5</v>
       </c>
+      <c r="AG68" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="AH68" s="13" t="s">
+        <v>235</v>
+      </c>
     </row>
-    <row r="69" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>177</v>
       </c>
@@ -9155,8 +9558,14 @@
       <c r="AF69">
         <v>3</v>
       </c>
+      <c r="AG69" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="AH69" s="14" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="70" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>179</v>
       </c>
@@ -9253,8 +9662,14 @@
       <c r="AF70">
         <v>4</v>
       </c>
+      <c r="AG70" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="AH70" s="13" t="s">
+        <v>226</v>
+      </c>
     </row>
-    <row r="71" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>181</v>
       </c>
@@ -9351,8 +9766,14 @@
       <c r="AF71">
         <v>3</v>
       </c>
+      <c r="AG71" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="AH71" s="14" t="s">
+        <v>221</v>
+      </c>
     </row>
-    <row r="72" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>182</v>
       </c>
@@ -9449,8 +9870,14 @@
       <c r="AF72">
         <v>1</v>
       </c>
+      <c r="AG72" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="AH72" s="13" t="s">
+        <v>222</v>
+      </c>
     </row>
-    <row r="73" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>184</v>
       </c>
@@ -9547,8 +9974,14 @@
       <c r="AF73">
         <v>5</v>
       </c>
+      <c r="AG73" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="AH73" s="14" t="s">
+        <v>223</v>
+      </c>
     </row>
-    <row r="74" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>185</v>
       </c>
@@ -9645,8 +10078,14 @@
       <c r="AF74">
         <v>3</v>
       </c>
+      <c r="AG74" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="AH74" s="13" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="75" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>186</v>
       </c>
@@ -9743,8 +10182,14 @@
       <c r="AF75">
         <v>6</v>
       </c>
+      <c r="AG75" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="AH75" s="14" t="s">
+        <v>217</v>
+      </c>
     </row>
-    <row r="76" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>187</v>
       </c>
@@ -9841,8 +10286,14 @@
       <c r="AF76">
         <v>5</v>
       </c>
+      <c r="AG76" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="AH76" s="13" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="77" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>188</v>
       </c>
@@ -9939,8 +10390,14 @@
       <c r="AF77">
         <v>2</v>
       </c>
+      <c r="AG77" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="AH77" s="14" t="s">
+        <v>223</v>
+      </c>
     </row>
-    <row r="78" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>189</v>
       </c>
@@ -10037,8 +10494,14 @@
       <c r="AF78">
         <v>0</v>
       </c>
+      <c r="AG78" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="AH78" s="13" t="s">
+        <v>222</v>
+      </c>
     </row>
-    <row r="79" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>190</v>
       </c>
@@ -10135,8 +10598,14 @@
       <c r="AF79">
         <v>1</v>
       </c>
+      <c r="AG79" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="AH79" s="14" t="s">
+        <v>232</v>
+      </c>
     </row>
-    <row r="80" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>191</v>
       </c>
@@ -10233,8 +10702,14 @@
       <c r="AF80">
         <v>2</v>
       </c>
+      <c r="AG80" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="AH80" s="13" t="s">
+        <v>231</v>
+      </c>
     </row>
-    <row r="81" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>192</v>
       </c>
@@ -10331,8 +10806,14 @@
       <c r="AF81">
         <v>4</v>
       </c>
+      <c r="AG81" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="AH81" s="14" t="s">
+        <v>214</v>
+      </c>
     </row>
-    <row r="82" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>193</v>
       </c>
@@ -10429,8 +10910,14 @@
       <c r="AF82">
         <v>4</v>
       </c>
+      <c r="AG82" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="AH82" s="13" t="s">
+        <v>214</v>
+      </c>
     </row>
-    <row r="83" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>194</v>
       </c>
@@ -10527,8 +11014,14 @@
       <c r="AF83">
         <v>3</v>
       </c>
+      <c r="AG83" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="AH83" s="14" t="s">
+        <v>224</v>
+      </c>
     </row>
-    <row r="84" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>195</v>
       </c>
@@ -10625,8 +11118,14 @@
       <c r="AF84">
         <v>4</v>
       </c>
+      <c r="AG84" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="AH84" s="13" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="85" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>196</v>
       </c>
@@ -10723,8 +11222,14 @@
       <c r="AF85">
         <v>3</v>
       </c>
+      <c r="AG85" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="AH85" s="14" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="86" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>197</v>
       </c>
@@ -10821,8 +11326,14 @@
       <c r="AF86">
         <v>5</v>
       </c>
+      <c r="AG86" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="AH86" s="13" t="s">
+        <v>216</v>
+      </c>
     </row>
-    <row r="87" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>198</v>
       </c>
@@ -10919,8 +11430,14 @@
       <c r="AF87">
         <v>4</v>
       </c>
+      <c r="AG87" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="AH87" s="14" t="s">
+        <v>214</v>
+      </c>
     </row>
-    <row r="88" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>199</v>
       </c>
@@ -11017,8 +11534,14 @@
       <c r="AF88">
         <v>4</v>
       </c>
+      <c r="AG88" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="AH88" s="13" t="s">
+        <v>222</v>
+      </c>
     </row>
-    <row r="89" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>200</v>
       </c>
@@ -11115,8 +11638,14 @@
       <c r="AF89">
         <v>8</v>
       </c>
+      <c r="AG89" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="AH89" s="14" t="s">
+        <v>225</v>
+      </c>
     </row>
-    <row r="90" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>201</v>
       </c>
@@ -11213,8 +11742,14 @@
       <c r="AF90">
         <v>2</v>
       </c>
+      <c r="AG90" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="AH90" s="13" t="s">
+        <v>224</v>
+      </c>
     </row>
-    <row r="91" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>202</v>
       </c>
@@ -11311,8 +11846,14 @@
       <c r="AF91">
         <v>9</v>
       </c>
+      <c r="AG91" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="AH91" s="14" t="s">
+        <v>223</v>
+      </c>
     </row>
-    <row r="92" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>203</v>
       </c>
@@ -11409,8 +11950,14 @@
       <c r="AF92">
         <v>4</v>
       </c>
+      <c r="AG92" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="AH92" s="13" t="s">
+        <v>214</v>
+      </c>
     </row>
-    <row r="93" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>204</v>
       </c>
@@ -11507,8 +12054,14 @@
       <c r="AF93">
         <v>1</v>
       </c>
+      <c r="AG93" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="AH93" s="14" t="s">
+        <v>215</v>
+      </c>
     </row>
-    <row r="94" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>205</v>
       </c>
@@ -11605,8 +12158,14 @@
       <c r="AF94">
         <v>5</v>
       </c>
+      <c r="AG94" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="AH94" s="13" t="s">
+        <v>220</v>
+      </c>
     </row>
-    <row r="95" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>206</v>
       </c>
@@ -11703,8 +12262,14 @@
       <c r="AF95">
         <v>8</v>
       </c>
+      <c r="AG95" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="AH95" s="14" t="s">
+        <v>216</v>
+      </c>
     </row>
-    <row r="96" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>207</v>
       </c>
@@ -11801,8 +12366,14 @@
       <c r="AF96">
         <v>5</v>
       </c>
+      <c r="AG96" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="AH96" s="13" t="s">
+        <v>218</v>
+      </c>
     </row>
-    <row r="97" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>184</v>
       </c>
@@ -11899,8 +12470,14 @@
       <c r="AF97">
         <v>8</v>
       </c>
+      <c r="AG97" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="AH97" s="14" t="s">
+        <v>214</v>
+      </c>
     </row>
-    <row r="100" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>25</v>
       </c>
@@ -12017,7 +12594,7 @@
         <v>3.4918032786885247</v>
       </c>
     </row>
-    <row r="101" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>26</v>
       </c>
@@ -12093,7 +12670,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="102" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:34" x14ac:dyDescent="0.2">
       <c r="H102" s="2">
         <f>H101/(H101+I101+J101)</f>
         <v>0.5846470185058259</v>
@@ -12155,13 +12732,13 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="105" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:34" x14ac:dyDescent="0.2">
       <c r="Y105" s="11" t="s">
         <v>29</v>
       </c>
       <c r="Z105" s="11"/>
     </row>
-    <row r="106" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:34" x14ac:dyDescent="0.2">
       <c r="H106" s="11" t="s">
         <v>27</v>
       </c>
@@ -12174,7 +12751,7 @@
       <c r="Y106" s="11"/>
       <c r="Z106" s="11"/>
     </row>
-    <row r="107" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:34" x14ac:dyDescent="0.2">
       <c r="H107" s="11"/>
       <c r="I107" s="11"/>
       <c r="J107" s="11"/>
@@ -12183,7 +12760,7 @@
       <c r="Y107" s="11"/>
       <c r="Z107" s="11"/>
     </row>
-    <row r="108" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:34" x14ac:dyDescent="0.2">
       <c r="H108" s="11"/>
       <c r="I108" s="11"/>
       <c r="J108" s="11"/>
@@ -12192,7 +12769,7 @@
       <c r="Y108" s="11"/>
       <c r="Z108" s="11"/>
     </row>
-    <row r="109" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:34" x14ac:dyDescent="0.2">
       <c r="Y109" s="11"/>
       <c r="Z109" s="11"/>
     </row>
@@ -12220,8 +12797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FDF367E-2F8F-BD4D-A310-A68FC9A48C26}">
   <dimension ref="A1:AH114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG26" sqref="AG26"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AG2" sqref="AG2:AH97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>